<commit_message>
updated fp: american, feather, san j, stan, yuba
</commit_message>
<xml_diff>
--- a/data-raw/floodplain/CVPIA_FloodplainAreas.xlsx
+++ b/data-raw/floodplain/CVPIA_FloodplainAreas.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MetaData" sheetId="1" state="visible" r:id="rId2"/>
@@ -591,27 +591,27 @@
   </sheetPr>
   <dimension ref="A1:Z35"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="T1" activeCellId="0" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.9230769230769"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.1376518218623"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.2064777327935"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="42.9554655870445"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.5263157894737"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="43.3846153846154"/>
     <col collapsed="false" hidden="false" max="6" min="5" style="0" width="14.1417004048583"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.5668016194332"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.7125506072875"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="15.6396761133603"/>
-    <col collapsed="false" hidden="false" max="13" min="11" style="0" width="14.5668016194332"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.1740890688259"/>
-    <col collapsed="false" hidden="false" max="21" min="15" style="0" width="14.5668016194332"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="17.7813765182186"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="14.5668016194332"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="36.2064777327935"/>
-    <col collapsed="false" hidden="false" max="1025" min="25" style="0" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="14.6761133603239"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.8178137651822"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="13" min="11" style="0" width="14.6761133603239"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="21" min="15" style="0" width="14.6761133603239"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="14.6761133603239"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="36.5263157894737"/>
+    <col collapsed="false" hidden="false" max="1025" min="25" style="0" width="14.6761133603239"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3983,9 +3983,9 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="14" min="2" style="0" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="14" min="2" style="0" width="21.7449392712551"/>
     <col collapsed="false" hidden="false" max="27" min="15" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="1025" min="28" style="0" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1025" min="28" style="0" width="14.6761133603239"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4542,9 +4542,9 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="14" min="2" style="0" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="14" min="2" style="0" width="21.7449392712551"/>
     <col collapsed="false" hidden="false" max="27" min="15" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="1025" min="28" style="0" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1025" min="28" style="0" width="14.6761133603239"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5328,9 +5328,9 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="14" min="2" style="0" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="14" min="2" style="0" width="21.7449392712551"/>
     <col collapsed="false" hidden="false" max="27" min="15" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="1025" min="28" style="0" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1025" min="28" style="0" width="14.6761133603239"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5733,9 +5733,9 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="21.7449392712551"/>
     <col collapsed="false" hidden="false" max="17" min="5" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="14.6761133603239"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6212,9 +6212,9 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="21.7449392712551"/>
     <col collapsed="false" hidden="false" max="17" min="5" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="14.6761133603239"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6581,21 +6581,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N36"/>
+  <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="14" min="2" style="0" width="21.5303643724696"/>
-    <col collapsed="false" hidden="false" max="27" min="15" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="1025" min="28" style="0" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="13" min="2" style="0" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="26" min="14" style="0" width="8.67611336032389"/>
+    <col collapsed="false" hidden="false" max="1025" min="27" style="0" width="14.6761133603239"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="11" t="s">
         <v>85</v>
       </c>
@@ -6611,13 +6611,12 @@
       <c r="G1" s="11"/>
       <c r="H1" s="11"/>
       <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
+      <c r="J1" s="2"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="11"/>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="M1" s="11"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>200</v>
       </c>
@@ -6628,9 +6627,7 @@
         <f aca="false">IF(B2-MetaData!$T$2&lt;0,0,B2-MetaData!$T$2)</f>
         <v>0</v>
       </c>
-      <c r="D2" s="14" t="n">
-        <v>0</v>
-      </c>
+      <c r="D2" s="13"/>
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
       <c r="G2" s="13"/>
@@ -6640,9 +6637,8 @@
       <c r="K2" s="13"/>
       <c r="L2" s="13"/>
       <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>1200</v>
       </c>
@@ -6653,9 +6649,7 @@
         <f aca="false">IF(B3-MetaData!$T$2&lt;0,0,B3-MetaData!$T$2)</f>
         <v>0</v>
       </c>
-      <c r="D3" s="14" t="n">
-        <v>0</v>
-      </c>
+      <c r="D3" s="13"/>
       <c r="E3" s="13"/>
       <c r="F3" s="13"/>
       <c r="G3" s="13"/>
@@ -6665,9 +6659,8 @@
       <c r="K3" s="13"/>
       <c r="L3" s="13"/>
       <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>2200</v>
       </c>
@@ -6678,9 +6671,7 @@
         <f aca="false">IF(B4-MetaData!$T$2&lt;0,0,B4-MetaData!$T$2)</f>
         <v>5.99825528</v>
       </c>
-      <c r="D4" s="14" t="n">
-        <v>5.99825528007341</v>
-      </c>
+      <c r="D4" s="13"/>
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>
@@ -6690,9 +6681,8 @@
       <c r="K4" s="13"/>
       <c r="L4" s="13"/>
       <c r="M4" s="13"/>
-      <c r="N4" s="13"/>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>3200</v>
       </c>
@@ -6703,9 +6693,7 @@
         <f aca="false">IF(B5-MetaData!$T$2&lt;0,0,B5-MetaData!$T$2)</f>
         <v>159.8806244</v>
       </c>
-      <c r="D5" s="14" t="n">
-        <v>159.880624426079</v>
-      </c>
+      <c r="D5" s="13"/>
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
       <c r="G5" s="13"/>
@@ -6715,9 +6703,8 @@
       <c r="K5" s="13"/>
       <c r="L5" s="13"/>
       <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>4200</v>
       </c>
@@ -6728,9 +6715,7 @@
         <f aca="false">IF(B6-MetaData!$T$2&lt;0,0,B6-MetaData!$T$2)</f>
         <v>228.0077135</v>
       </c>
-      <c r="D6" s="14" t="n">
-        <v>228.007713498623</v>
-      </c>
+      <c r="D6" s="13"/>
       <c r="E6" s="13"/>
       <c r="F6" s="13"/>
       <c r="G6" s="13"/>
@@ -6740,9 +6725,8 @@
       <c r="K6" s="13"/>
       <c r="L6" s="13"/>
       <c r="M6" s="13"/>
-      <c r="N6" s="13"/>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>5200</v>
       </c>
@@ -6753,9 +6737,7 @@
         <f aca="false">IF(B7-MetaData!$T$2&lt;0,0,B7-MetaData!$T$2)</f>
         <v>268.523944</v>
       </c>
-      <c r="D7" s="14" t="n">
-        <v>268.523943985308</v>
-      </c>
+      <c r="D7" s="13"/>
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
       <c r="G7" s="13"/>
@@ -6765,9 +6747,8 @@
       <c r="K7" s="13"/>
       <c r="L7" s="13"/>
       <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>5570</v>
       </c>
@@ -6778,9 +6759,7 @@
         <f aca="false">IF(B8-MetaData!$T$2&lt;0,0,B8-MetaData!$T$2)</f>
         <v>294.3103873</v>
       </c>
-      <c r="D8" s="14" t="n">
-        <v>294.31038728191</v>
-      </c>
+      <c r="D8" s="13"/>
       <c r="E8" s="13"/>
       <c r="F8" s="13"/>
       <c r="G8" s="13"/>
@@ -6790,9 +6769,8 @@
       <c r="K8" s="13"/>
       <c r="L8" s="13"/>
       <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>6200</v>
       </c>
@@ -6803,9 +6781,7 @@
         <f aca="false">IF(B9-MetaData!$T$2&lt;0,0,B9-MetaData!$T$2)</f>
         <v>338.217034</v>
       </c>
-      <c r="D9" s="14" t="n">
-        <v>338.217033976125</v>
-      </c>
+      <c r="D9" s="13"/>
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
       <c r="G9" s="13"/>
@@ -6815,9 +6791,8 @@
       <c r="K9" s="13"/>
       <c r="L9" s="13"/>
       <c r="M9" s="13"/>
-      <c r="N9" s="13"/>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>7200</v>
       </c>
@@ -6828,9 +6803,7 @@
         <f aca="false">IF(B10-MetaData!$T$2&lt;0,0,B10-MetaData!$T$2)</f>
         <v>390.1414141</v>
       </c>
-      <c r="D10" s="14" t="n">
-        <v>390.141414141414</v>
-      </c>
+      <c r="D10" s="13"/>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
       <c r="G10" s="13"/>
@@ -6840,9 +6813,8 @@
       <c r="K10" s="13"/>
       <c r="L10" s="13"/>
       <c r="M10" s="13"/>
-      <c r="N10" s="13"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>8200</v>
       </c>
@@ -6853,9 +6825,7 @@
         <f aca="false">IF(B11-MetaData!$T$2&lt;0,0,B11-MetaData!$T$2)</f>
         <v>454.7623508</v>
       </c>
-      <c r="D11" s="14" t="n">
-        <v>454.762350780533</v>
-      </c>
+      <c r="D11" s="13"/>
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
@@ -6865,9 +6835,8 @@
       <c r="K11" s="13"/>
       <c r="L11" s="13"/>
       <c r="M11" s="13"/>
-      <c r="N11" s="13"/>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>9200</v>
       </c>
@@ -6878,9 +6847,7 @@
         <f aca="false">IF(B12-MetaData!$T$2&lt;0,0,B12-MetaData!$T$2)</f>
         <v>499.8296832</v>
       </c>
-      <c r="D12" s="14" t="n">
-        <v>499.829683195592</v>
-      </c>
+      <c r="D12" s="13"/>
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
       <c r="G12" s="13"/>
@@ -6890,9 +6857,8 @@
       <c r="K12" s="13"/>
       <c r="L12" s="13"/>
       <c r="M12" s="13"/>
-      <c r="N12" s="13"/>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>10200</v>
       </c>
@@ -6903,9 +6869,7 @@
         <f aca="false">IF(B13-MetaData!$T$2&lt;0,0,B13-MetaData!$T$2)</f>
         <v>534.6504591</v>
       </c>
-      <c r="D13" s="14" t="n">
-        <v>534.650459136823</v>
-      </c>
+      <c r="D13" s="13"/>
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
@@ -6915,9 +6879,8 @@
       <c r="K13" s="13"/>
       <c r="L13" s="13"/>
       <c r="M13" s="13"/>
-      <c r="N13" s="13"/>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>11200</v>
       </c>
@@ -6928,9 +6891,7 @@
         <f aca="false">IF(B14-MetaData!$T$2&lt;0,0,B14-MetaData!$T$2)</f>
         <v>568.7528237</v>
       </c>
-      <c r="D14" s="14" t="n">
-        <v>568.75282369146</v>
-      </c>
+      <c r="D14" s="13"/>
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
       <c r="G14" s="13"/>
@@ -6940,9 +6901,8 @@
       <c r="K14" s="13"/>
       <c r="L14" s="13"/>
       <c r="M14" s="13"/>
-      <c r="N14" s="13"/>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>12200</v>
       </c>
@@ -6953,9 +6913,7 @@
         <f aca="false">IF(B15-MetaData!$T$2&lt;0,0,B15-MetaData!$T$2)</f>
         <v>597.8565657</v>
       </c>
-      <c r="D15" s="14" t="n">
-        <v>597.856565656566</v>
-      </c>
+      <c r="D15" s="13"/>
       <c r="E15" s="13"/>
       <c r="F15" s="13"/>
       <c r="G15" s="13"/>
@@ -6965,9 +6923,8 @@
       <c r="K15" s="13"/>
       <c r="L15" s="13"/>
       <c r="M15" s="13"/>
-      <c r="N15" s="13"/>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <v>13200</v>
       </c>
@@ -6978,9 +6935,7 @@
         <f aca="false">IF(B16-MetaData!$T$2&lt;0,0,B16-MetaData!$T$2)</f>
         <v>622.5967401</v>
       </c>
-      <c r="D16" s="14" t="n">
-        <v>622.596740128558</v>
-      </c>
+      <c r="D16" s="13"/>
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
       <c r="G16" s="13"/>
@@ -6990,9 +6945,8 @@
       <c r="K16" s="13"/>
       <c r="L16" s="13"/>
       <c r="M16" s="13"/>
-      <c r="N16" s="13"/>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>14200</v>
       </c>
@@ -7003,9 +6957,7 @@
         <f aca="false">IF(B17-MetaData!$T$2&lt;0,0,B17-MetaData!$T$2)</f>
         <v>647.0566345</v>
       </c>
-      <c r="D17" s="14" t="n">
-        <v>647.056634527089</v>
-      </c>
+      <c r="D17" s="13"/>
       <c r="E17" s="13"/>
       <c r="F17" s="13"/>
       <c r="G17" s="13"/>
@@ -7015,9 +6967,8 @@
       <c r="K17" s="13"/>
       <c r="L17" s="13"/>
       <c r="M17" s="13"/>
-      <c r="N17" s="13"/>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
         <v>15200</v>
       </c>
@@ -7028,9 +6979,7 @@
         <f aca="false">IF(B18-MetaData!$T$2&lt;0,0,B18-MetaData!$T$2)</f>
         <v>672.8754362</v>
       </c>
-      <c r="D18" s="14" t="n">
-        <v>672.875436179982</v>
-      </c>
+      <c r="D18" s="13"/>
       <c r="E18" s="13"/>
       <c r="F18" s="13"/>
       <c r="G18" s="13"/>
@@ -7040,9 +6989,8 @@
       <c r="K18" s="13"/>
       <c r="L18" s="13"/>
       <c r="M18" s="13"/>
-      <c r="N18" s="13"/>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
         <v>16200</v>
       </c>
@@ -7053,9 +7001,7 @@
         <f aca="false">IF(B19-MetaData!$T$2&lt;0,0,B19-MetaData!$T$2)</f>
         <v>704.8254591</v>
       </c>
-      <c r="D19" s="14" t="n">
-        <v>704.825459136823</v>
-      </c>
+      <c r="D19" s="13"/>
       <c r="E19" s="13"/>
       <c r="F19" s="13"/>
       <c r="G19" s="13"/>
@@ -7065,9 +7011,8 @@
       <c r="K19" s="13"/>
       <c r="L19" s="13"/>
       <c r="M19" s="13"/>
-      <c r="N19" s="13"/>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
         <v>17200</v>
       </c>
@@ -7078,9 +7023,7 @@
         <f aca="false">IF(B20-MetaData!$T$2&lt;0,0,B20-MetaData!$T$2)</f>
         <v>729.6570478</v>
       </c>
-      <c r="D20" s="14" t="n">
-        <v>729.65704775023</v>
-      </c>
+      <c r="D20" s="13"/>
       <c r="E20" s="13"/>
       <c r="F20" s="13"/>
       <c r="G20" s="13"/>
@@ -7090,9 +7033,8 @@
       <c r="K20" s="13"/>
       <c r="L20" s="13"/>
       <c r="M20" s="13"/>
-      <c r="N20" s="13"/>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
         <v>18200</v>
       </c>
@@ -7103,9 +7045,7 @@
         <f aca="false">IF(B21-MetaData!$T$2&lt;0,0,B21-MetaData!$T$2)</f>
         <v>750.9006198</v>
       </c>
-      <c r="D21" s="14" t="n">
-        <v>750.900619834711</v>
-      </c>
+      <c r="D21" s="13"/>
       <c r="E21" s="13"/>
       <c r="F21" s="13"/>
       <c r="G21" s="13"/>
@@ -7115,9 +7055,8 @@
       <c r="K21" s="13"/>
       <c r="L21" s="13"/>
       <c r="M21" s="13"/>
-      <c r="N21" s="13"/>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
         <v>19200</v>
       </c>
@@ -7128,9 +7067,7 @@
         <f aca="false">IF(B22-MetaData!$T$2&lt;0,0,B22-MetaData!$T$2)</f>
         <v>776.2978191</v>
       </c>
-      <c r="D22" s="14" t="n">
-        <v>776.297819100092</v>
-      </c>
+      <c r="D22" s="13"/>
       <c r="E22" s="13"/>
       <c r="F22" s="13"/>
       <c r="G22" s="13"/>
@@ -7140,9 +7077,8 @@
       <c r="K22" s="13"/>
       <c r="L22" s="13"/>
       <c r="M22" s="13"/>
-      <c r="N22" s="13"/>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
         <v>20200</v>
       </c>
@@ -7153,9 +7089,7 @@
         <f aca="false">IF(B23-MetaData!$T$2&lt;0,0,B23-MetaData!$T$2)</f>
         <v>800.1617769</v>
       </c>
-      <c r="D23" s="14" t="n">
-        <v>800.161776859504</v>
-      </c>
+      <c r="D23" s="13"/>
       <c r="E23" s="13"/>
       <c r="F23" s="13"/>
       <c r="G23" s="13"/>
@@ -7165,9 +7099,8 @@
       <c r="K23" s="13"/>
       <c r="L23" s="13"/>
       <c r="M23" s="13"/>
-      <c r="N23" s="13"/>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
         <v>21200</v>
       </c>
@@ -7178,9 +7111,7 @@
         <f aca="false">IF(B24-MetaData!$T$2&lt;0,0,B24-MetaData!$T$2)</f>
         <v>826.4326676</v>
       </c>
-      <c r="D24" s="14" t="n">
-        <v>826.43266758494</v>
-      </c>
+      <c r="D24" s="13"/>
       <c r="E24" s="13"/>
       <c r="F24" s="13"/>
       <c r="G24" s="13"/>
@@ -7190,9 +7121,8 @@
       <c r="K24" s="13"/>
       <c r="L24" s="13"/>
       <c r="M24" s="13"/>
-      <c r="N24" s="13"/>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
         <v>22200</v>
       </c>
@@ -7203,9 +7133,7 @@
         <f aca="false">IF(B25-MetaData!$T$2&lt;0,0,B25-MetaData!$T$2)</f>
         <v>846.7327824</v>
       </c>
-      <c r="D25" s="14" t="n">
-        <v>846.732782369146</v>
-      </c>
+      <c r="D25" s="13"/>
       <c r="E25" s="13"/>
       <c r="F25" s="13"/>
       <c r="G25" s="13"/>
@@ -7215,9 +7143,8 @@
       <c r="K25" s="13"/>
       <c r="L25" s="13"/>
       <c r="M25" s="13"/>
-      <c r="N25" s="13"/>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
         <v>23200</v>
       </c>
@@ -7228,9 +7155,7 @@
         <f aca="false">IF(B26-MetaData!$T$2&lt;0,0,B26-MetaData!$T$2)</f>
         <v>862.5653811</v>
       </c>
-      <c r="D26" s="14" t="n">
-        <v>862.565381083563</v>
-      </c>
+      <c r="D26" s="13"/>
       <c r="E26" s="13"/>
       <c r="F26" s="13"/>
       <c r="G26" s="13"/>
@@ -7240,9 +7165,8 @@
       <c r="K26" s="13"/>
       <c r="L26" s="13"/>
       <c r="M26" s="13"/>
-      <c r="N26" s="13"/>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
         <v>24200</v>
       </c>
@@ -7253,9 +7177,7 @@
         <f aca="false">IF(B27-MetaData!$T$2&lt;0,0,B27-MetaData!$T$2)</f>
         <v>880.6505739</v>
       </c>
-      <c r="D27" s="14" t="n">
-        <v>880.650573921028</v>
-      </c>
+      <c r="D27" s="13"/>
       <c r="E27" s="13"/>
       <c r="F27" s="13"/>
       <c r="G27" s="13"/>
@@ -7265,9 +7187,8 @@
       <c r="K27" s="13"/>
       <c r="L27" s="13"/>
       <c r="M27" s="13"/>
-      <c r="N27" s="13"/>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
         <v>25200</v>
       </c>
@@ -7278,9 +7199,7 @@
         <f aca="false">IF(B28-MetaData!$T$2&lt;0,0,B28-MetaData!$T$2)</f>
         <v>900.4679752</v>
       </c>
-      <c r="D28" s="14" t="n">
-        <v>900.467975206612</v>
-      </c>
+      <c r="D28" s="13"/>
       <c r="E28" s="13"/>
       <c r="F28" s="13"/>
       <c r="G28" s="13"/>
@@ -7290,9 +7209,8 @@
       <c r="K28" s="13"/>
       <c r="L28" s="13"/>
       <c r="M28" s="13"/>
-      <c r="N28" s="13"/>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
         <v>26200</v>
       </c>
@@ -7303,9 +7221,7 @@
         <f aca="false">IF(B29-MetaData!$T$2&lt;0,0,B29-MetaData!$T$2)</f>
         <v>919.2378099</v>
       </c>
-      <c r="D29" s="14" t="n">
-        <v>919.237809917355</v>
-      </c>
+      <c r="D29" s="13"/>
       <c r="E29" s="13"/>
       <c r="F29" s="13"/>
       <c r="G29" s="13"/>
@@ -7315,9 +7231,8 @@
       <c r="K29" s="13"/>
       <c r="L29" s="13"/>
       <c r="M29" s="13"/>
-      <c r="N29" s="13"/>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
         <v>27200</v>
       </c>
@@ -7328,9 +7243,7 @@
         <f aca="false">IF(B30-MetaData!$T$2&lt;0,0,B30-MetaData!$T$2)</f>
         <v>937.7069789</v>
       </c>
-      <c r="D30" s="14" t="n">
-        <v>937.706978879706</v>
-      </c>
+      <c r="D30" s="13"/>
       <c r="E30" s="13"/>
       <c r="F30" s="13"/>
       <c r="G30" s="13"/>
@@ -7340,9 +7253,8 @@
       <c r="K30" s="13"/>
       <c r="L30" s="13"/>
       <c r="M30" s="13"/>
-      <c r="N30" s="13"/>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
         <v>28200</v>
       </c>
@@ -7353,9 +7265,7 @@
         <f aca="false">IF(B31-MetaData!$T$2&lt;0,0,B31-MetaData!$T$2)</f>
         <v>953.5370753</v>
       </c>
-      <c r="D31" s="14" t="n">
-        <v>953.537075298439</v>
-      </c>
+      <c r="D31" s="13"/>
       <c r="E31" s="13"/>
       <c r="F31" s="13"/>
       <c r="G31" s="13"/>
@@ -7365,9 +7275,8 @@
       <c r="K31" s="13"/>
       <c r="L31" s="13"/>
       <c r="M31" s="13"/>
-      <c r="N31" s="13"/>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
         <v>29200</v>
       </c>
@@ -7378,9 +7287,7 @@
         <f aca="false">IF(B32-MetaData!$T$2&lt;0,0,B32-MetaData!$T$2)</f>
         <v>969.0983395</v>
       </c>
-      <c r="D32" s="14" t="n">
-        <v>969.098339455157</v>
-      </c>
+      <c r="D32" s="13"/>
       <c r="E32" s="13"/>
       <c r="F32" s="13"/>
       <c r="G32" s="13"/>
@@ -7389,9 +7296,8 @@
       <c r="J32" s="13"/>
       <c r="K32" s="13"/>
       <c r="L32" s="13"/>
-      <c r="M32" s="13"/>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
         <v>30200</v>
       </c>
@@ -7402,9 +7308,7 @@
         <f aca="false">IF(B33-MetaData!$T$2&lt;0,0,B33-MetaData!$T$2)</f>
         <v>984.6596036</v>
       </c>
-      <c r="D33" s="14" t="n">
-        <v>984.659603611876</v>
-      </c>
+      <c r="D33" s="13"/>
       <c r="E33" s="13"/>
       <c r="F33" s="13"/>
       <c r="G33" s="13"/>
@@ -7413,9 +7317,8 @@
       <c r="J33" s="13"/>
       <c r="K33" s="13"/>
       <c r="L33" s="13"/>
-      <c r="M33" s="13"/>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
         <v>31200</v>
       </c>
@@ -7426,9 +7329,7 @@
         <f aca="false">IF(B34-MetaData!$T$2&lt;0,0,B34-MetaData!$T$2)</f>
         <v>1000.220868</v>
       </c>
-      <c r="D34" s="14" t="n">
-        <v>1000.2208677686</v>
-      </c>
+      <c r="D34" s="13"/>
       <c r="E34" s="13"/>
       <c r="F34" s="13"/>
       <c r="G34" s="13"/>
@@ -7437,9 +7338,8 @@
       <c r="J34" s="13"/>
       <c r="K34" s="13"/>
       <c r="L34" s="13"/>
-      <c r="M34" s="13"/>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
         <v>32200</v>
       </c>
@@ -7450,9 +7350,7 @@
         <f aca="false">IF(B35-MetaData!$T$2&lt;0,0,B35-MetaData!$T$2)</f>
         <v>1016.309435</v>
       </c>
-      <c r="D35" s="14" t="n">
-        <v>1016.30943526171</v>
-      </c>
+      <c r="D35" s="13"/>
       <c r="E35" s="13"/>
       <c r="F35" s="13"/>
       <c r="G35" s="13"/>
@@ -7461,9 +7359,8 @@
       <c r="J35" s="13"/>
       <c r="K35" s="13"/>
       <c r="L35" s="13"/>
-      <c r="M35" s="13"/>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
         <v>33200</v>
       </c>
@@ -7474,9 +7371,7 @@
         <f aca="false">IF(B36-MetaData!$T$2&lt;0,0,B36-MetaData!$T$2)</f>
         <v>1032.398003</v>
       </c>
-      <c r="D36" s="14" t="n">
-        <v>1032.39800275482</v>
-      </c>
+      <c r="D36" s="13"/>
       <c r="E36" s="13"/>
       <c r="F36" s="13"/>
       <c r="G36" s="13"/>
@@ -7485,7 +7380,6 @@
       <c r="J36" s="13"/>
       <c r="K36" s="13"/>
       <c r="L36" s="13"/>
-      <c r="M36" s="13"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -7512,9 +7406,9 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="21.7449392712551"/>
     <col collapsed="false" hidden="false" max="17" min="5" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="14.6761133603239"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7956,9 +7850,9 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="21.7449392712551"/>
     <col collapsed="false" hidden="false" max="17" min="5" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="14.6761133603239"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8472,9 +8366,9 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="21.7449392712551"/>
     <col collapsed="false" hidden="false" max="17" min="5" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="14.6761133603239"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8916,9 +8810,9 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="14" min="2" style="0" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="14" min="2" style="0" width="21.7449392712551"/>
     <col collapsed="false" hidden="false" max="27" min="15" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="1025" min="28" style="0" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1025" min="28" style="0" width="14.6761133603239"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9704,9 +9598,9 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="14" min="2" style="0" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="14" min="2" style="0" width="21.7449392712551"/>
     <col collapsed="false" hidden="false" max="27" min="15" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="1025" min="28" style="0" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1025" min="28" style="0" width="14.6761133603239"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10447,9 +10341,9 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="14" min="2" style="0" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="14" min="2" style="0" width="21.7449392712551"/>
     <col collapsed="false" hidden="false" max="27" min="15" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="1025" min="28" style="0" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1025" min="28" style="0" width="14.6761133603239"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11211,9 +11105,9 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="14" min="2" style="0" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="14" min="2" style="0" width="21.7449392712551"/>
     <col collapsed="false" hidden="false" max="27" min="15" style="0" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="1025" min="28" style="0" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1025" min="28" style="0" width="14.6761133603239"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="27" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>